<commit_message>
complete fixing of tests; removed unneeded test files
</commit_message>
<xml_diff>
--- a/tests/data_files/workbooks/Exp_HiC_insert.xlsx
+++ b/tests/data_files/workbooks/Exp_HiC_insert.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10615"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrew/Documents/work/Submit4DN/tests/data_files/workbooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7E5CDC33-0CDC-D147-A5AF-E549B16C35CD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E653FFD4-546C-E14A-BC01-850C6BB2DF91}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32760" yWindow="1880" windowWidth="25040" windowHeight="15500"/>
+    <workbookView xWindow="1580" yWindow="1360" windowWidth="25040" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ExperimentHiC" sheetId="1" r:id="rId1"/>
@@ -352,7 +352,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -795,13 +795,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:AK104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AB1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="AG2" sqref="AG2"/>
     </sheetView>
   </sheetViews>

</xml_diff>